<commit_message>
word format draft of the ctFIRE web page
</commit_message>
<xml_diff>
--- a/ctFIRE/FIREdefparam.xlsx
+++ b/ctFIRE/FIREdefparam.xlsx
@@ -54,9 +54,6 @@
     <t>thresh_im2</t>
   </si>
   <si>
-    <t>thresh_im2 is for a hard value, main adjustable parameters</t>
-  </si>
-  <si>
     <t>thresh_Dxlink</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>s_fiberdir</t>
   </si>
   <si>
-    <t>distance for linknig same-oriented fibers</t>
-  </si>
-  <si>
     <t>thresh_linkd</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>angle similarity required for a fiber to extend to the next point(cos(70*pi/180))</t>
   </si>
   <si>
-    <t>maximum dangle angler difference at cross-link(cos(10*pi/180))</t>
-  </si>
-  <si>
     <t>minimum angle between two fiber ends for linking of the two fibers(cos(-150 *pi/180))</t>
   </si>
   <si>
@@ -199,6 +190,15 @@
   </si>
   <si>
     <t>[1 1 1]</t>
+  </si>
+  <si>
+    <t>distance for linking similarly-oriented fibers</t>
+  </si>
+  <si>
+    <t>a grey level threshold value used for initially converting the image to a binary image prior to the distance transform</t>
+  </si>
+  <si>
+    <t>maximum dangler angle difference at cross-link(cos(10*pi/180))</t>
   </si>
 </sst>
 </file>
@@ -532,14 +532,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -561,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>0.3</v>
@@ -578,13 +579,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="O3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -615,7 +616,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
         <v>1</v>
@@ -626,13 +627,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -640,13 +641,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -654,13 +655,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>0.2</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -668,13 +669,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
         <v>0</v>
@@ -685,13 +686,13 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -699,13 +700,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0.5</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -713,13 +714,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -727,13 +728,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -741,13 +742,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -755,13 +756,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -769,13 +770,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -783,13 +784,13 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -797,13 +798,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -811,13 +812,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>-150</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -825,13 +826,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20">
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -839,13 +840,13 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -853,13 +854,13 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -867,13 +868,13 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -881,13 +882,13 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -895,13 +896,13 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -909,13 +910,13 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26">
         <v>0.01</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -923,13 +924,13 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="10:10">

</xml_diff>

<commit_message>
append the parameters for curvelet transform
</commit_message>
<xml_diff>
--- a/ctFIRE/FIREdefparam.xlsx
+++ b/ctFIRE/FIREdefparam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="14355" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="16275" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
-  <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+  <si>
+    <t>sigma_im</t>
+  </si>
+  <si>
+    <t>sigma_d</t>
+  </si>
+  <si>
+    <t>dtype</t>
+  </si>
+  <si>
+    <t>thresh_im</t>
+  </si>
+  <si>
+    <t>thresh_im2</t>
+  </si>
+  <si>
+    <t>thresh_Dxlink</t>
+  </si>
+  <si>
+    <t>s_xlinkbox</t>
+  </si>
+  <si>
+    <t>thresh_LMP</t>
+  </si>
+  <si>
+    <t>thresh_LMPdist</t>
+  </si>
+  <si>
+    <t>thresh_ext</t>
+  </si>
+  <si>
+    <t>lam_dirdecay</t>
+  </si>
+  <si>
+    <t>s_minstep</t>
+  </si>
+  <si>
+    <t>s_maxstep</t>
+  </si>
+  <si>
+    <t>thresh_dang_aextend</t>
+  </si>
+  <si>
+    <t>thresh_dang_L</t>
+  </si>
+  <si>
+    <t>thresh_short_L</t>
+  </si>
+  <si>
+    <t>s_fiberdir</t>
+  </si>
+  <si>
+    <t>thresh_linkd</t>
+  </si>
+  <si>
+    <t>thresh_linka</t>
+  </si>
+  <si>
+    <t>thresh_flen</t>
+  </si>
+  <si>
+    <t>thresh_numv</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>s_boundthick</t>
+  </si>
+  <si>
+    <t>blist</t>
+  </si>
+  <si>
+    <t>s_maxspace</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>ang_interval</t>
+  </si>
+  <si>
+    <t>pct</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>cityblock</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1 1]</t>
   </si>
   <si>
     <t>radius of box for smoothing original image</t>
@@ -33,55 +120,28 @@
     <t>radius of box for smoothing of distance function</t>
   </si>
   <si>
-    <t>sigma_im</t>
-  </si>
-  <si>
-    <t>dtype</t>
-  </si>
-  <si>
     <t>type of distance transform for bwdist ; cityblock is significantly faster than Euclidean distance)</t>
   </si>
   <si>
-    <t>thresh_im</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
     <t>thresh_im  is for a percentage of maximum</t>
   </si>
   <si>
-    <t>thresh_im2</t>
-  </si>
-  <si>
-    <t>thresh_Dxlink</t>
+    <t>thresh_im2 is for a hard value, main adjustable parameters</t>
   </si>
   <si>
     <t>dist fun. threshold for a point to be considered an x-link</t>
   </si>
   <si>
-    <t>thresh_LMP</t>
+    <t>radius of box in which to check to make sure xlink is a local max of the distance function</t>
   </si>
   <si>
     <t>threshold for a point to be considered an LMP</t>
   </si>
   <si>
-    <t>radius of box in which to check to make sure xlink is a local max of the distance function</t>
-  </si>
-  <si>
-    <t>s_xlinkbox</t>
-  </si>
-  <si>
-    <t>thresh_LMPdist</t>
-  </si>
-  <si>
     <t>minimum distance apart for two LMPs</t>
   </si>
   <si>
-    <t>thresh_ext</t>
-  </si>
-  <si>
-    <t>lam_dirdecay</t>
+    <t>angle similarity required for a fiber to extend to the next point(cos(70*pi/180))</t>
   </si>
   <si>
     <t>decay rate of fiber direction (to make it more difficult for a fiber to turn around)</t>
@@ -90,78 +150,42 @@
     <t>minimum step size</t>
   </si>
   <si>
-    <t>s_minstep</t>
-  </si>
-  <si>
     <t>max step size</t>
   </si>
   <si>
-    <t>s_maxstep</t>
-  </si>
-  <si>
-    <t>thresh_dang_aextend</t>
-  </si>
-  <si>
-    <t>thresh_dang_L</t>
-  </si>
-  <si>
-    <t>thresh_short_L</t>
+    <t>maximum dangle angler difference at cross-link(cos(10*pi/180))</t>
+  </si>
+  <si>
+    <t>dangler length threshold</t>
+  </si>
+  <si>
+    <t>short fiber length threshold</t>
   </si>
   <si>
     <t>number of nodes used for claculating direction of fiber end</t>
   </si>
   <si>
-    <t>s_fiberdir</t>
-  </si>
-  <si>
-    <t>thresh_linkd</t>
-  </si>
-  <si>
-    <t>thresh_linka</t>
+    <t>distance for linknig same-oriented fibers</t>
+  </si>
+  <si>
+    <t>minimum angle between two fiber ends for linking of the two fibers(cos(-150 *pi/180))</t>
   </si>
   <si>
     <t>minimum length of a free fiber</t>
   </si>
   <si>
-    <t>thresh_flen</t>
-  </si>
-  <si>
     <t>minimum number of verties a free fiber can have</t>
   </si>
   <si>
-    <t>thresh_numv</t>
-  </si>
-  <si>
-    <t>scale</t>
+    <t>change x,y,z scale([.05 .05 .1])</t>
   </si>
   <si>
     <t>pixels of thickness for image boundary</t>
   </si>
   <si>
-    <t>s_boundthick</t>
-  </si>
-  <si>
     <t xml:space="preserve">indicates which boundaries are controlled (1=x,2=y,3=z) </t>
   </si>
   <si>
-    <t>blist</t>
-  </si>
-  <si>
-    <t>s_maxspace</t>
-  </si>
-  <si>
-    <t>lambda</t>
-  </si>
-  <si>
-    <t>ang_interval</t>
-  </si>
-  <si>
-    <t>dangler length threshold</t>
-  </si>
-  <si>
-    <t>short fiber length threshold</t>
-  </si>
-  <si>
     <t>maximum spacing between vertices along a fiber</t>
   </si>
   <si>
@@ -171,34 +195,10 @@
     <t>interval for caculate angle at each point</t>
   </si>
   <si>
-    <t>sigma_d</t>
-  </si>
-  <si>
-    <t>cityblock</t>
-  </si>
-  <si>
-    <t>no 'cityblock'</t>
-  </si>
-  <si>
-    <t>angle similarity required for a fiber to extend to the next point(cos(70*pi/180))</t>
-  </si>
-  <si>
-    <t>minimum angle between two fiber ends for linking of the two fibers(cos(-150 *pi/180))</t>
-  </si>
-  <si>
-    <t>change x,y,z scale([.05 .05 .1])</t>
-  </si>
-  <si>
-    <t>[1 1 1]</t>
-  </si>
-  <si>
-    <t>distance for linking similarly-oriented fibers</t>
-  </si>
-  <si>
-    <t>a grey level threshold value used for initially converting the image to a binary image prior to the distance transform</t>
-  </si>
-  <si>
-    <t>maximum dangler angle difference at cross-link(cos(10*pi/180))</t>
+    <t>Percentile of the remaining curvelet coeffs</t>
+  </si>
+  <si>
+    <t>Number of selected scales</t>
   </si>
 </sst>
 </file>
@@ -530,233 +530,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0.3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>0.2</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>0.5</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -765,12 +752,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -784,13 +771,13 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -798,13 +785,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -812,13 +799,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>-150</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -826,13 +813,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -840,13 +827,13 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -854,13 +841,13 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -868,13 +855,13 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -882,13 +869,13 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -896,13 +883,13 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -910,13 +897,13 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>0.01</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -924,23 +911,45 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="10:10">
-      <c r="J41" t="s">
-        <v>2</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>0.2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
correct a spelling error
</commit_message>
<xml_diff>
--- a/ctFIRE/FIREdefparam.xlsx
+++ b/ctFIRE/FIREdefparam.xlsx
@@ -162,9 +162,6 @@
     <t>short fiber length threshold</t>
   </si>
   <si>
-    <t>number of nodes used for claculating direction of fiber end</t>
-  </si>
-  <si>
     <t>distance for linknig same-oriented fibers</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Number of selected scales</t>
+  </si>
+  <si>
+    <t>number of nodes used for calculating direction of fiber end</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -777,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -791,7 +791,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -805,7 +805,7 @@
         <v>-150</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -819,7 +819,7 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -833,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -847,7 +847,7 @@
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -861,7 +861,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -889,7 +889,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -903,7 +903,7 @@
         <v>0.01</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -917,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -931,7 +931,7 @@
         <v>0.2</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -945,7 +945,7 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>